<commit_message>
Redid prov indicators; added elasticity analysis
</commit_message>
<xml_diff>
--- a/data_summary/data_summary_by_stat.xlsx
+++ b/data_summary/data_summary_by_stat.xlsx
@@ -105,7 +105,7 @@
     <t>Latest Census Pop. (CMP)</t>
   </si>
   <si>
-    <t>Provider_PPSA</t>
+    <t>Provider_MPSA</t>
   </si>
   <si>
     <t>Provider_Municipal</t>
@@ -212,7 +212,7 @@
     <tableColumn id="25" name="Biennial Surplus/Capita (REV)" dataDxfId="0"/>
     <tableColumn id="26" name="Total Non-Warrant Rev./Capita (REV)" dataDxfId="0"/>
     <tableColumn id="27" name="Latest Census Pop. (CMP)" dataDxfId="0"/>
-    <tableColumn id="28" name="Provider_PPSA" dataDxfId="0"/>
+    <tableColumn id="28" name="Provider_MPSA" dataDxfId="0"/>
     <tableColumn id="29" name="Provider_Municipal" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -250,7 +250,7 @@
     <tableColumn id="25" name="Biennial Surplus/Capita (REV)" dataDxfId="0"/>
     <tableColumn id="26" name="Total Non-Warrant Rev./Capita (REV)" dataDxfId="0"/>
     <tableColumn id="27" name="Latest Census Pop. (CMP)" dataDxfId="0"/>
-    <tableColumn id="28" name="Provider_PPSA" dataDxfId="0"/>
+    <tableColumn id="28" name="Provider_MPSA" dataDxfId="0"/>
     <tableColumn id="29" name="Provider_Municipal" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -288,7 +288,7 @@
     <tableColumn id="25" name="Biennial Surplus/Capita (REV)" dataDxfId="1"/>
     <tableColumn id="26" name="Total Non-Warrant Rev./Capita (REV)" dataDxfId="1"/>
     <tableColumn id="27" name="Latest Census Pop. (CMP)" dataDxfId="1"/>
-    <tableColumn id="28" name="Provider_PPSA" dataDxfId="1"/>
+    <tableColumn id="28" name="Provider_MPSA" dataDxfId="1"/>
     <tableColumn id="29" name="Provider_Municipal" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -326,7 +326,7 @@
     <tableColumn id="25" name="Biennial Surplus/Capita (REV)" dataDxfId="1"/>
     <tableColumn id="26" name="Total Non-Warrant Rev./Capita (REV)" dataDxfId="1"/>
     <tableColumn id="27" name="Latest Census Pop. (CMP)" dataDxfId="1"/>
-    <tableColumn id="28" name="Provider_PPSA" dataDxfId="1"/>
+    <tableColumn id="28" name="Provider_MPSA" dataDxfId="1"/>
     <tableColumn id="29" name="Provider_Municipal" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -364,7 +364,7 @@
     <tableColumn id="25" name="Biennial Surplus/Capita (REV)" dataDxfId="1"/>
     <tableColumn id="26" name="Total Non-Warrant Rev./Capita (REV)" dataDxfId="1"/>
     <tableColumn id="27" name="Latest Census Pop. (CMP)" dataDxfId="0"/>
-    <tableColumn id="28" name="Provider_PPSA" dataDxfId="0"/>
+    <tableColumn id="28" name="Provider_MPSA" dataDxfId="0"/>
     <tableColumn id="29" name="Provider_Municipal" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -402,7 +402,7 @@
     <tableColumn id="25" name="Biennial Surplus/Capita (REV)" dataDxfId="1"/>
     <tableColumn id="26" name="Total Non-Warrant Rev./Capita (REV)" dataDxfId="1"/>
     <tableColumn id="27" name="Latest Census Pop. (CMP)" dataDxfId="1"/>
-    <tableColumn id="28" name="Provider_PPSA" dataDxfId="1"/>
+    <tableColumn id="28" name="Provider_MPSA" dataDxfId="1"/>
     <tableColumn id="29" name="Provider_Municipal" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -440,7 +440,7 @@
     <tableColumn id="25" name="Biennial Surplus/Capita (REV)" dataDxfId="1"/>
     <tableColumn id="26" name="Total Non-Warrant Rev./Capita (REV)" dataDxfId="1"/>
     <tableColumn id="27" name="Latest Census Pop. (CMP)" dataDxfId="1"/>
-    <tableColumn id="28" name="Provider_PPSA" dataDxfId="1"/>
+    <tableColumn id="28" name="Provider_MPSA" dataDxfId="1"/>
     <tableColumn id="29" name="Provider_Municipal" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -478,7 +478,7 @@
     <tableColumn id="25" name="Biennial Surplus/Capita (REV)" dataDxfId="1"/>
     <tableColumn id="26" name="Total Non-Warrant Rev./Capita (REV)" dataDxfId="1"/>
     <tableColumn id="27" name="Latest Census Pop. (CMP)" dataDxfId="1"/>
-    <tableColumn id="28" name="Provider_PPSA" dataDxfId="1"/>
+    <tableColumn id="28" name="Provider_MPSA" dataDxfId="1"/>
     <tableColumn id="29" name="Provider_Municipal" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -516,7 +516,7 @@
     <tableColumn id="25" name="Biennial Surplus/Capita (REV)" dataDxfId="1"/>
     <tableColumn id="26" name="Total Non-Warrant Rev./Capita (REV)" dataDxfId="1"/>
     <tableColumn id="27" name="Latest Census Pop. (CMP)" dataDxfId="0"/>
-    <tableColumn id="28" name="Provider_PPSA" dataDxfId="0"/>
+    <tableColumn id="28" name="Provider_MPSA" dataDxfId="0"/>
     <tableColumn id="29" name="Provider_Municipal" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -841,7 +841,7 @@
     <col min="25" max="25" width="29.28515625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="35.7109375" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="17" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2579,7 +2579,7 @@
     <col min="25" max="25" width="29.28515625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="35.7109375" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="17" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4317,7 +4317,7 @@
     <col min="25" max="25" width="29.28515625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="35.7109375" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="19" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="20" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4493,7 +4493,7 @@
         <v>4447.514563106796</v>
       </c>
       <c r="AB2" s="3">
-        <v>0.7281553398058253</v>
+        <v>0.116504854368932</v>
       </c>
       <c r="AC2" s="3">
         <v>0.1553398058252427</v>
@@ -4582,7 +4582,7 @@
         <v>4447.514563106796</v>
       </c>
       <c r="AB3" s="3">
-        <v>0.7281553398058253</v>
+        <v>0.116504854368932</v>
       </c>
       <c r="AC3" s="3">
         <v>0.1553398058252427</v>
@@ -4671,7 +4671,7 @@
         <v>4447.514563106796</v>
       </c>
       <c r="AB4" s="3">
-        <v>0.7281553398058253</v>
+        <v>0.116504854368932</v>
       </c>
       <c r="AC4" s="3">
         <v>0.1553398058252427</v>
@@ -4760,7 +4760,7 @@
         <v>4397.902912621359</v>
       </c>
       <c r="AB5" s="3">
-        <v>0.7281553398058253</v>
+        <v>0.116504854368932</v>
       </c>
       <c r="AC5" s="3">
         <v>0.1553398058252427</v>
@@ -4849,7 +4849,7 @@
         <v>4397.902912621359</v>
       </c>
       <c r="AB6" s="3">
-        <v>0.7281553398058253</v>
+        <v>0.116504854368932</v>
       </c>
       <c r="AC6" s="3">
         <v>0.1553398058252427</v>
@@ -4938,7 +4938,7 @@
         <v>4397.902912621359</v>
       </c>
       <c r="AB7" s="3">
-        <v>0.7281553398058253</v>
+        <v>0.116504854368932</v>
       </c>
       <c r="AC7" s="3">
         <v>0.1553398058252427</v>
@@ -5027,7 +5027,7 @@
         <v>4476.872549019608</v>
       </c>
       <c r="AB8" s="3">
-        <v>0.7352941176470589</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="AC8" s="3">
         <v>0.1470588235294118</v>
@@ -5116,7 +5116,7 @@
         <v>4476.872549019608</v>
       </c>
       <c r="AB9" s="3">
-        <v>0.7352941176470589</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="AC9" s="3">
         <v>0.1470588235294118</v>
@@ -5205,7 +5205,7 @@
         <v>4528.673267326732</v>
       </c>
       <c r="AB10" s="3">
-        <v>0.7326732673267327</v>
+        <v>0.1188118811881188</v>
       </c>
       <c r="AC10" s="3">
         <v>0.1485148514851485</v>
@@ -5294,7 +5294,7 @@
         <v>4528.673267326732</v>
       </c>
       <c r="AB11" s="3">
-        <v>0.7326732673267327</v>
+        <v>0.1188118811881188</v>
       </c>
       <c r="AC11" s="3">
         <v>0.1485148514851485</v>
@@ -5383,7 +5383,7 @@
         <v>4528.673267326732</v>
       </c>
       <c r="AB12" s="3">
-        <v>0.7326732673267327</v>
+        <v>0.1188118811881188</v>
       </c>
       <c r="AC12" s="3">
         <v>0.1485148514851485</v>
@@ -5472,7 +5472,7 @@
         <v>4742.792079207921</v>
       </c>
       <c r="AB13" s="3">
-        <v>0.7326732673267327</v>
+        <v>0.1188118811881188</v>
       </c>
       <c r="AC13" s="3">
         <v>0.1485148514851485</v>
@@ -5561,7 +5561,7 @@
         <v>4781.87</v>
       </c>
       <c r="AB14" s="3">
-        <v>0.73</v>
+        <v>0.12</v>
       </c>
       <c r="AC14" s="3">
         <v>0.15</v>
@@ -5650,7 +5650,7 @@
         <v>4783.83</v>
       </c>
       <c r="AB15" s="3">
-        <v>0.73</v>
+        <v>0.12</v>
       </c>
       <c r="AC15" s="3">
         <v>0.15</v>
@@ -5739,7 +5739,7 @@
         <v>4782.323232323232</v>
       </c>
       <c r="AB16" s="3">
-        <v>0.7272727272727273</v>
+        <v>0.1212121212121212</v>
       </c>
       <c r="AC16" s="3">
         <v>0.1515151515151515</v>
@@ -5828,7 +5828,7 @@
         <v>4824.151515151515</v>
       </c>
       <c r="AB17" s="3">
-        <v>0.7272727272727273</v>
+        <v>0.1212121212121212</v>
       </c>
       <c r="AC17" s="3">
         <v>0.1515151515151515</v>
@@ -5917,7 +5917,7 @@
         <v>4824.151515151515</v>
       </c>
       <c r="AB18" s="3">
-        <v>0.7272727272727273</v>
+        <v>0.1212121212121212</v>
       </c>
       <c r="AC18" s="3">
         <v>0.1515151515151515</v>
@@ -6006,7 +6006,7 @@
         <v>5010.336842105263</v>
       </c>
       <c r="AB19" s="3">
-        <v>0.7157894736842105</v>
+        <v>0.1263157894736842</v>
       </c>
       <c r="AC19" s="3">
         <v>0.1578947368421053</v>
@@ -6231,7 +6231,7 @@
         <v>10478.49171984332</v>
       </c>
       <c r="AB2" s="3">
-        <v>0.4470858749217429</v>
+        <v>0.3223982093132047</v>
       </c>
       <c r="AC2" s="3">
         <v>0.3639996108971757</v>
@@ -6320,7 +6320,7 @@
         <v>10478.49171984332</v>
       </c>
       <c r="AB3" s="3">
-        <v>0.4470858749217429</v>
+        <v>0.3223982093132047</v>
       </c>
       <c r="AC3" s="3">
         <v>0.3639996108971757</v>
@@ -6409,7 +6409,7 @@
         <v>10478.49171984332</v>
       </c>
       <c r="AB4" s="3">
-        <v>0.4470858749217429</v>
+        <v>0.3223982093132047</v>
       </c>
       <c r="AC4" s="3">
         <v>0.3639996108971757</v>
@@ -6498,7 +6498,7 @@
         <v>10418.83796022675</v>
       </c>
       <c r="AB5" s="3">
-        <v>0.4470858749217429</v>
+        <v>0.3223982093132047</v>
       </c>
       <c r="AC5" s="3">
         <v>0.3639996108971757</v>
@@ -6587,7 +6587,7 @@
         <v>10418.83796022675</v>
       </c>
       <c r="AB6" s="3">
-        <v>0.4470858749217429</v>
+        <v>0.3223982093132047</v>
       </c>
       <c r="AC6" s="3">
         <v>0.3639996108971757</v>
@@ -6676,7 +6676,7 @@
         <v>10418.83796022676</v>
       </c>
       <c r="AB7" s="3">
-        <v>0.4470858749217428</v>
+        <v>0.3223982093132048</v>
       </c>
       <c r="AC7" s="3">
         <v>0.3639996108971757</v>
@@ -6765,7 +6765,7 @@
         <v>10716.09086186903</v>
       </c>
       <c r="AB8" s="3">
-        <v>0.4433551330755756</v>
+        <v>0.3237808098282633</v>
       </c>
       <c r="AC8" s="3">
         <v>0.3559135177948392</v>
@@ -6854,7 +6854,7 @@
         <v>10716.09086186903</v>
       </c>
       <c r="AB9" s="3">
-        <v>0.4433551330755756</v>
+        <v>0.3237808098282633</v>
       </c>
       <c r="AC9" s="3">
         <v>0.3559135177948392</v>
@@ -6943,7 +6943,7 @@
         <v>10757.99855094702</v>
       </c>
       <c r="AB10" s="3">
-        <v>0.4447716067581403</v>
+        <v>0.3251808331642962</v>
       </c>
       <c r="AC10" s="3">
         <v>0.3573832288695536</v>
@@ -7032,7 +7032,7 @@
         <v>10757.99855094702</v>
       </c>
       <c r="AB11" s="3">
-        <v>0.4447716067581403</v>
+        <v>0.3251808331642962</v>
       </c>
       <c r="AC11" s="3">
         <v>0.3573832288695536</v>
@@ -7121,7 +7121,7 @@
         <v>10757.99855094702</v>
       </c>
       <c r="AB12" s="3">
-        <v>0.4447716067581404</v>
+        <v>0.3251808331642962</v>
       </c>
       <c r="AC12" s="3">
         <v>0.3573832288695536</v>
@@ -7210,7 +7210,7 @@
         <v>11508.34640712282</v>
       </c>
       <c r="AB13" s="3">
-        <v>0.4447716067581404</v>
+        <v>0.3251808331642962</v>
       </c>
       <c r="AC13" s="3">
         <v>0.3573832288695536</v>
@@ -7299,7 +7299,7 @@
         <v>11559.59530648006</v>
       </c>
       <c r="AB14" s="3">
-        <v>0.4461960433384737</v>
+        <v>0.3265986323710905</v>
       </c>
       <c r="AC14" s="3">
         <v>0.3588702812826368</v>
@@ -7388,7 +7388,7 @@
         <v>11558.87649468117</v>
       </c>
       <c r="AB15" s="3">
-        <v>0.4461960433384737</v>
+        <v>0.3265986323710905</v>
       </c>
       <c r="AC15" s="3">
         <v>0.3588702812826368</v>
@@ -7477,7 +7477,7 @@
         <v>11617.69080275131</v>
       </c>
       <c r="AB16" s="3">
-        <v>0.4476282581717946</v>
+        <v>0.328034569878314</v>
       </c>
       <c r="AC16" s="3">
         <v>0.3603749850782236</v>
@@ -7566,7 +7566,7 @@
         <v>11778.20489801676</v>
       </c>
       <c r="AB17" s="3">
-        <v>0.4476282581717946</v>
+        <v>0.328034569878314</v>
       </c>
       <c r="AC17" s="3">
         <v>0.3603749850782236</v>
@@ -7655,7 +7655,7 @@
         <v>11778.20489801676</v>
       </c>
       <c r="AB18" s="3">
-        <v>0.4476282581717946</v>
+        <v>0.328034569878314</v>
       </c>
       <c r="AC18" s="3">
         <v>0.3603749850782236</v>
@@ -7744,7 +7744,7 @@
         <v>12011.39351280162</v>
       </c>
       <c r="AB19" s="3">
-        <v>0.4534303740855227</v>
+        <v>0.333967295607331</v>
       </c>
       <c r="AC19" s="3">
         <v>0.3665767306309685</v>
@@ -7793,7 +7793,7 @@
     <col min="25" max="25" width="29.28515625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="35.7109375" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="17" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -9531,7 +9531,7 @@
     <col min="25" max="25" width="29.28515625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="35.7109375" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="17" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -11269,7 +11269,7 @@
     <col min="25" max="25" width="29.28515625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="35.7109375" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="17" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -11445,7 +11445,7 @@
         <v>1379</v>
       </c>
       <c r="AB2" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC2" s="3">
         <v>0</v>
@@ -11534,7 +11534,7 @@
         <v>1379</v>
       </c>
       <c r="AB3" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC3" s="3">
         <v>0</v>
@@ -11623,7 +11623,7 @@
         <v>1379</v>
       </c>
       <c r="AB4" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC4" s="3">
         <v>0</v>
@@ -11712,7 +11712,7 @@
         <v>1335</v>
       </c>
       <c r="AB5" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC5" s="3">
         <v>0</v>
@@ -11801,7 +11801,7 @@
         <v>1335</v>
       </c>
       <c r="AB6" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC6" s="3">
         <v>0</v>
@@ -11890,7 +11890,7 @@
         <v>1335</v>
       </c>
       <c r="AB7" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC7" s="3">
         <v>0</v>
@@ -11979,7 +11979,7 @@
         <v>1291.5</v>
       </c>
       <c r="AB8" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC8" s="3">
         <v>0</v>
@@ -12068,7 +12068,7 @@
         <v>1291.5</v>
       </c>
       <c r="AB9" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC9" s="3">
         <v>0</v>
@@ -12157,7 +12157,7 @@
         <v>1314</v>
       </c>
       <c r="AB10" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC10" s="3">
         <v>0</v>
@@ -12246,7 +12246,7 @@
         <v>1314</v>
       </c>
       <c r="AB11" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC11" s="3">
         <v>0</v>
@@ -12335,7 +12335,7 @@
         <v>1314</v>
       </c>
       <c r="AB12" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC12" s="3">
         <v>0</v>
@@ -12424,7 +12424,7 @@
         <v>1286</v>
       </c>
       <c r="AB13" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC13" s="3">
         <v>0</v>
@@ -12513,7 +12513,7 @@
         <v>1293.5</v>
       </c>
       <c r="AB14" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC14" s="3">
         <v>0</v>
@@ -12602,7 +12602,7 @@
         <v>1293.5</v>
       </c>
       <c r="AB15" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC15" s="3">
         <v>0</v>
@@ -12691,7 +12691,7 @@
         <v>1286</v>
       </c>
       <c r="AB16" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC16" s="3">
         <v>0</v>
@@ -12780,7 +12780,7 @@
         <v>1285</v>
       </c>
       <c r="AB17" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC17" s="3">
         <v>0</v>
@@ -12869,7 +12869,7 @@
         <v>1285</v>
       </c>
       <c r="AB18" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC18" s="3">
         <v>0</v>
@@ -12958,7 +12958,7 @@
         <v>1305</v>
       </c>
       <c r="AB19" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC19" s="3">
         <v>0</v>
@@ -13007,7 +13007,7 @@
     <col min="25" max="25" width="29.28515625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="35.7109375" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="17" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -13183,7 +13183,7 @@
         <v>4081</v>
       </c>
       <c r="AB2" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC2" s="3">
         <v>0</v>
@@ -13272,7 +13272,7 @@
         <v>4081</v>
       </c>
       <c r="AB3" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC3" s="3">
         <v>0</v>
@@ -13361,7 +13361,7 @@
         <v>4081</v>
       </c>
       <c r="AB4" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC4" s="3">
         <v>0</v>
@@ -13450,7 +13450,7 @@
         <v>3975</v>
       </c>
       <c r="AB5" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC5" s="3">
         <v>0</v>
@@ -13539,7 +13539,7 @@
         <v>3975</v>
       </c>
       <c r="AB6" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC6" s="3">
         <v>0</v>
@@ -13628,7 +13628,7 @@
         <v>3975</v>
       </c>
       <c r="AB7" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC7" s="3">
         <v>0</v>
@@ -13717,7 +13717,7 @@
         <v>3676</v>
       </c>
       <c r="AB8" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC8" s="3">
         <v>0</v>
@@ -13806,7 +13806,7 @@
         <v>3676</v>
       </c>
       <c r="AB9" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC9" s="3">
         <v>0</v>
@@ -13895,7 +13895,7 @@
         <v>3676</v>
       </c>
       <c r="AB10" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC10" s="3">
         <v>0</v>
@@ -13984,7 +13984,7 @@
         <v>3676</v>
       </c>
       <c r="AB11" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC11" s="3">
         <v>0</v>
@@ -14073,7 +14073,7 @@
         <v>3676</v>
       </c>
       <c r="AB12" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC12" s="3">
         <v>0</v>
@@ -14162,7 +14162,7 @@
         <v>3512</v>
       </c>
       <c r="AB13" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC13" s="3">
         <v>0</v>
@@ -14251,7 +14251,7 @@
         <v>3512</v>
       </c>
       <c r="AB14" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC14" s="3">
         <v>0</v>
@@ -14340,7 +14340,7 @@
         <v>3512</v>
       </c>
       <c r="AB15" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC15" s="3">
         <v>0</v>
@@ -14429,7 +14429,7 @@
         <v>3512</v>
       </c>
       <c r="AB16" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC16" s="3">
         <v>0</v>
@@ -14518,7 +14518,7 @@
         <v>3570</v>
       </c>
       <c r="AB17" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC17" s="3">
         <v>0</v>
@@ -14607,7 +14607,7 @@
         <v>3570</v>
       </c>
       <c r="AB18" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC18" s="3">
         <v>0</v>
@@ -14696,7 +14696,7 @@
         <v>4174</v>
       </c>
       <c r="AB19" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC19" s="3">
         <v>0</v>
@@ -14745,7 +14745,7 @@
     <col min="25" max="25" width="29.28515625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="35.7109375" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="17" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>